<commit_message>
bulk upload file change
</commit_message>
<xml_diff>
--- a/MDO/client-assets/assets/common/users-file-upload-sample.xlsx
+++ b/MDO/client-assets/assets/common/users-file-upload-sample.xlsx
@@ -1,47 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26522"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26611"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurav\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AC70103-5F32-4C26-8C8C-0FD2560511A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_E46F02CA63F5329F3750BA89C655F65AD2BC8B01" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7311328C-3CC2-4382-A573-CD63A7AF875D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+  <si>
+    <t>Full Name</t>
   </si>
   <si>
     <t>Email Id</t>
@@ -60,23 +41,61 @@
   </si>
   <si>
     <t>External Reference System</t>
+  </si>
+  <si>
+    <t>New User</t>
+  </si>
+  <si>
+    <t>new_user01@yopmail.com</t>
+  </si>
+  <si>
+    <t>Contractual Staff</t>
+  </si>
+  <si>
+    <t>southwest,s2</t>
+  </si>
+  <si>
+    <t>USER123</t>
+  </si>
+  <si>
+    <t>USERABC</t>
+  </si>
+  <si>
+    <t>new_user03@yopmail.com</t>
+  </si>
+  <si>
+    <t>Group B</t>
+  </si>
+  <si>
+    <t>s1,s2</t>
+  </si>
+  <si>
+    <t>newuser_08@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -120,18 +139,89 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFCE4D6"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0563C1"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -439,19 +529,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AB659A-788E-42FA-AA49-4E47406AB9C7}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E409" sqref="E409"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7" ht="13.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,16 +571,78 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="13.9">
+      <c r="A2" t="s">
         <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8688586858</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.9">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>8688885858</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.85">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>8688585858</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E421" xr:uid="{8BD4366F-DACE-4453-B467-284AE2FFDFD3}">
-      <formula1>"Group A,Group B,Group C,Group D,Contractual Staff, Others"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"Group A,Group B,Group C,Group D,Contractual Staff"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes in mdo assets
</commit_message>
<xml_diff>
--- a/MDO/client-assets/assets/common/users-file-upload-sample.xlsx
+++ b/MDO/client-assets/assets/common/users-file-upload-sample.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26903"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_E46F02CA63F5329F3750BA89C655F65AD2BC8B01" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A28BF55F-71E3-44BF-9344-22CD0930E010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="1E-4"/>
+  <definedNames>
+    <definedName name="NameValidation">Sheet1!$I$1:$I$1</definedName>
+  </definedNames>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -20,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Full Name</t>
   </si>
@@ -46,7 +63,7 @@
     <t>New User</t>
   </si>
   <si>
-    <t>new_user01@yopmail.com</t>
+    <t>new_user01@yopmail.coco</t>
   </si>
   <si>
     <t>Contractual Staff</t>
@@ -61,16 +78,10 @@
     <t>USERABC</t>
   </si>
   <si>
-    <t>new_user03@yopmail.com</t>
-  </si>
-  <si>
     <t>Group B</t>
   </si>
   <si>
     <t>s1,s2</t>
-  </si>
-  <si>
-    <t>newuser_08@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -530,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -572,7 +583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.9">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -580,7 +591,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>8688586858</v>
+        <v>9698989969</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -600,16 +611,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>9698989969</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
-        <v>8688885858</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -620,10 +631,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>8688585858</v>
+        <v>9698989969</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -632,15 +643,64 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:7">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="2"/>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="5">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter valid mobile number" error="Enter valid mobile number" promptTitle="Enter valid mobile number" prompt="Enter valid mobile number" sqref="C2:C4 C6:C1048576" xr:uid="{716210EB-9F99-4B94-A70B-A943099A3B83}">
+      <formula1>AND(ISNUMBER(C2), LEN(C2) =10)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{893D6942-5A49-4C1E-82C0-F918EDF6E104}">
       <formula1>"Group A,Group B,Group C,Group D,Contractual Staff"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter Valid Name" error="Name can contain only characters and space" promptTitle="Enter Valid Name" prompt="Name can contain only characters and space" sqref="A2:A1048576" xr:uid="{79873DE1-D166-4863-9273-CCCED7104E04}">
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(A2,ROW(INDIRECT("1:"&amp;LEN(A2))),1),"abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ ")))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter valid email" error="Enter valid email" promptTitle="Enter valid email" prompt="Enter valid email" sqref="B2:B1048576" xr:uid="{D267198A-2537-4759-AF08-4E6A2CA59313}">
+      <formula1>AND(ISERROR(FIND(" ",B2)),LEN(B2)-LEN(SUBSTITUTE(B2,"@",""))=1,IFERROR(SEARCH("@",B2)&lt;SEARCH(".",B2,SEARCH("@",B2)),0),ISERROR(FIND(",",B2)),NOT(IFERROR(SEARCH(".",B2,SEARCH("@",B2))-SEARCH("@",B2),0)=1),LEFT(B2,1)&lt;&gt;".",RIGHT(B2,1)&lt;&gt;".")</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576 C5" xr:uid="{C9FD5F64-95E7-45B8-9F6D-A826D3CC5E57}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F889DD2C-ACF5-4022-9AEA-84220A095848}"/>
+    <hyperlink ref="B3:B4" r:id="rId2" xr:uid="{F12DB452-EF36-48A4-854F-838C3CF4F66F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>